<commit_message>
************************************************* * This commit provide changes: 1. To run tests on both IE and Chrome * ************************************************* * Changes are made to: 1. testng.xml *include tests for IE 2. Baseclass.java *ammend method instantiatebrowser *ammend if statements for browsers 3. Loginpage.java *change driver find element by xpath to cssselector 4. LoginpageScript.java *ammend code *************************************************
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5FD318-E579-4A0D-8586-FF0BB5ACC3B2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1BC23778-843B-408E-8AB4-E077F058CE02}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="2484" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,10 +29,10 @@
     <t>demo</t>
   </si>
   <si>
-    <t>validuname</t>
+    <t>santhi.asusvivobook@gmail.com</t>
   </si>
   <si>
-    <t>validpwd</t>
+    <t>santhi_asusvivobook</t>
   </si>
 </sst>
 </file>
@@ -363,7 +364,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -388,10 +389,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="santhiparambalam@gmail.com" xr:uid="{9F090268-5D31-4882-82D4-46A2B6F5CDA8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>